<commit_message>
Fixed ClassData not getting committed
</commit_message>
<xml_diff>
--- a/data/mock data.xlsx
+++ b/data/mock data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e6ec02417029431/!CLASS NOTES/Fall 2022/Capstone/TeamMicrosoftPaint/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{84A2D83B-6208-47B4-9166-42728E5E883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C63D1774-FF0C-4658-95F5-D4ACF66F4AD6}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{84A2D83B-6208-47B4-9166-42728E5E883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24D753A4-8D2C-46E5-B515-1508ED7A872C}"/>
   <bookViews>
     <workbookView xWindow="4770" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -558,7 +558,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added admin page functionality, missing sample data
</commit_message>
<xml_diff>
--- a/data/mock data.xlsx
+++ b/data/mock data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e6ec02417029431/!CLASS NOTES/Fall 2022/Capstone/TeamMicrosoftPaint/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{84A2D83B-6208-47B4-9166-42728E5E883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C63D1774-FF0C-4658-95F5-D4ACF66F4AD6}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{84A2D83B-6208-47B4-9166-42728E5E883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{246B3E3E-8BC6-485F-98BA-0D141393CB23}"/>
   <bookViews>
     <workbookView xWindow="4770" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
   <si>
     <t>Program Code</t>
   </si>
@@ -228,6 +228,57 @@
   </si>
   <si>
     <t>Major College GPA</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Cena</t>
+  </si>
+  <si>
+    <t>Wrestling</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Intro to Wrestling</t>
+  </si>
+  <si>
+    <t>Wrestling 2</t>
+  </si>
+  <si>
+    <t>WES1001</t>
+  </si>
+  <si>
+    <t>WES1002</t>
+  </si>
+  <si>
+    <t>Top Rope Jumping</t>
+  </si>
+  <si>
+    <t>WES4955</t>
+  </si>
+  <si>
+    <t>Wresting Capstone</t>
+  </si>
+  <si>
+    <t>WES9999</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C-</t>
   </si>
 </sst>
 </file>
@@ -555,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,6 +728,110 @@
         <v>2022</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>125687</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>125687</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>125687</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>125687</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8">
+        <v>2021</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -687,7 +842,7 @@
   <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,7 +987,54 @@
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="O3" s="2"/>
+      <c r="A3">
+        <v>125687</v>
+      </c>
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="M3" t="s">
+        <v>70</v>
+      </c>
+      <c r="N3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="2">
+        <v>44338</v>
+      </c>
+      <c r="P3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3">
+        <v>158</v>
+      </c>
+      <c r="R3">
+        <v>2.9</v>
+      </c>
+      <c r="S3">
+        <v>2.99</v>
+      </c>
+      <c r="T3">
+        <v>3.54</v>
+      </c>
+      <c r="U3">
+        <v>800</v>
+      </c>
+      <c r="V3">
+        <v>21</v>
+      </c>
+      <c r="W3" t="s">
+        <v>71</v>
+      </c>
+      <c r="X3" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="O5" s="2"/>
@@ -845,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3977F79-6E6B-4605-81D9-CDEF365CEB35}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -926,6 +1128,20 @@
         <v>52</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>125687</v>
+      </c>
+      <c r="B3">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>198</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Linked front-end and back-end
</commit_message>
<xml_diff>
--- a/data/mock data.xlsx
+++ b/data/mock data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e6ec02417029431/!CLASS NOTES/Fall 2022/Capstone/TeamMicrosoftPaint/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="8_{84A2D83B-6208-47B4-9166-42728E5E883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{246B3E3E-8BC6-485F-98BA-0D141393CB23}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="8_{84A2D83B-6208-47B4-9166-42728E5E883C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DA5A6B4-7074-40F2-8B5C-610ACFD3E12B}"/>
   <bookViews>
-    <workbookView xWindow="4770" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="class_data" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="102">
   <si>
     <t>Program Code</t>
   </si>
@@ -279,6 +279,60 @@
   </si>
   <si>
     <t>C-</t>
+  </si>
+  <si>
+    <t>Rathbun</t>
+  </si>
+  <si>
+    <t>Jared</t>
+  </si>
+  <si>
+    <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>Cyber Security</t>
+  </si>
+  <si>
+    <t>Problem Solving w/ Java</t>
+  </si>
+  <si>
+    <t>CSC1610</t>
+  </si>
+  <si>
+    <t>Data Structures</t>
+  </si>
+  <si>
+    <t>CSC2820</t>
+  </si>
+  <si>
+    <t>Object Oriented Design</t>
+  </si>
+  <si>
+    <t>CSC2620</t>
+  </si>
+  <si>
+    <t>Analysis of Algorithms</t>
+  </si>
+  <si>
+    <t>CSC2710</t>
+  </si>
+  <si>
+    <t>Network Security</t>
+  </si>
+  <si>
+    <t>CSC5055</t>
+  </si>
+  <si>
+    <t>Web Development</t>
+  </si>
+  <si>
+    <t>CSC3222</t>
+  </si>
+  <si>
+    <t>Computer Science Capstone</t>
+  </si>
+  <si>
+    <t>CSC3333</t>
   </si>
 </sst>
 </file>
@@ -606,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -832,6 +886,188 @@
         <v>2021</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>789456</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>789456</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>789456</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>789456</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>789456</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>789456</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>789456</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15">
+        <v>2022</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -841,8 +1077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE02928E-DFB3-44AA-A9AE-F8BE7E05EDF9}">
   <dimension ref="A1:X5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1033,6 +1269,56 @@
         <v>71</v>
       </c>
       <c r="X3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>789456</v>
+      </c>
+      <c r="B4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" t="s">
+        <v>70</v>
+      </c>
+      <c r="N4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4">
+        <v>7</v>
+      </c>
+      <c r="R4">
+        <v>1.2</v>
+      </c>
+      <c r="S4">
+        <v>2.1</v>
+      </c>
+      <c r="T4">
+        <v>3.99</v>
+      </c>
+      <c r="U4">
+        <v>400</v>
+      </c>
+      <c r="V4">
+        <v>2</v>
+      </c>
+      <c r="W4" t="s">
+        <v>48</v>
+      </c>
+      <c r="X4" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>